<commit_message>
Changes for Estimation engine for Low level Estimations
</commit_message>
<xml_diff>
--- a/src/Estimation.xlsx
+++ b/src/Estimation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation_Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Estimation_LL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Simple</t>
   </si>
@@ -45,6 +46,27 @@
   </si>
   <si>
     <t>Final_Tech_LOE</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Trans</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple </t>
   </si>
 </sst>
 </file>
@@ -392,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -631,4 +653,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>